<commit_message>
added screws to coilcube bom
</commit_message>
<xml_diff>
--- a/assembly/coilcube/assembly_bom.xlsx
+++ b/assembly/coilcube/assembly_bom.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Manufacturer Part Number</t>
   </si>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t>Epoxy</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>#4 3/16" Panhead Self-Tapping Screws</t>
   </si>
 </sst>
 </file>
@@ -609,188 +615,230 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="56" customWidth="1"/>
+    <col min="2" max="2" width="26.5" customWidth="1"/>
+    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="2" t="s">
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="2" t="s">
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="1"/>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>2</v>
+      </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>